<commit_message>
22/11/2022 - 17h25 - fin journée
</commit_message>
<xml_diff>
--- a/Exercices/01 - Persistance des données/03 - Remplir les tableaux/03 - StagiairesAFPA/stagiaireAfpa.xlsx
+++ b/Exercices/01 - Persistance des données/03 - Remplir les tableaux/03 - StagiairesAFPA/stagiaireAfpa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\01 - Persistance des données\03 - Remplir les tableaux\03 - StagiairesAFPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8B6CA-534C-4AF6-BE25-4E96BAA4BABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345C3352-77E2-4D68-9CE5-9B1CC4584010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="116">
   <si>
     <t>adresse</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>21-34-56-78</t>
   </si>
 </sst>
 </file>
@@ -1315,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AW16" sqref="AW16"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,8 +1485,8 @@
       <c r="F2" s="4">
         <v>62100</v>
       </c>
-      <c r="G2" s="4">
-        <v>21345678</v>
+      <c r="G2" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="H2" s="5">
         <v>41883</v>
@@ -1516,8 +1519,8 @@
         <v>2</v>
       </c>
       <c r="Q2" s="13" t="str">
-        <f>"INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("""&amp;B2&amp;""", """&amp;C2&amp;""", """&amp;D2&amp;""", """&amp;E2&amp;""", "&amp;F2&amp;", """&amp;G2&amp;""", """&amp;TEXT(H2,"aaaa-mm-jj")&amp;""", """&amp;I2&amp;""", """&amp;TEXT(J2,"aaaa-mm-jj")&amp;""", "&amp;L2&amp;", "&amp;N2&amp;", "&amp;P2&amp;");"</f>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("roblin", "lea", "12,bd de la liberte", "calais", 62100, "21345678", "2014-09-01", "F", "1995-01-14", 5, 2, 2);</v>
+        <f>"INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("""&amp;B2&amp;""", """&amp;C2&amp;""", """&amp;D2&amp;""", """&amp;E2&amp;""", "&amp;F2&amp;", ""03-"&amp;G2&amp;""", """&amp;TEXT(H2,"aaaa-mm-jj")&amp;""", """&amp;I2&amp;""", """&amp;TEXT(J2,"aaaa-mm-jj")&amp;""", "&amp;L2&amp;", "&amp;N2&amp;", "&amp;P2&amp;");"</f>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("roblin", "lea", "12,bd de la liberte", "calais", 62100, "03-21-34-56-78", "2014-09-01", "F", "1995-01-14", 5, 2, 2);</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>79</v>
@@ -1597,11 +1600,11 @@
       </c>
       <c r="AV2">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AW2" t="str">
         <f ca="1">"INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES ("&amp;AT2&amp;", "&amp;AU2&amp;", "&amp;AV2&amp;");"</f>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (1, 2, 7);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (1, 2, 3);</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
@@ -1657,8 +1660,8 @@
         <v>2</v>
       </c>
       <c r="Q3" s="13" t="str">
-        <f t="shared" ref="Q3:Q19" si="2">"INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("""&amp;B3&amp;""", """&amp;C3&amp;""", """&amp;D3&amp;""", """&amp;E3&amp;""", "&amp;F3&amp;", """&amp;G3&amp;""", """&amp;TEXT(H3,"aaaa-mm-jj")&amp;""", """&amp;I3&amp;""", """&amp;TEXT(J3,"aaaa-mm-jj")&amp;""", "&amp;L3&amp;", "&amp;N3&amp;", "&amp;P3&amp;");"</f>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("macarthur", "leon", "121,bd gambetta", "calais", 62100, "21-30-65-09", "2014-09-01", "M", "1994-04-12", 3, 1, 2);</v>
+        <f t="shared" ref="Q3:Q19" si="2">"INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("""&amp;B3&amp;""", """&amp;C3&amp;""", """&amp;D3&amp;""", """&amp;E3&amp;""", "&amp;F3&amp;", ""03-"&amp;G3&amp;""", """&amp;TEXT(H3,"aaaa-mm-jj")&amp;""", """&amp;I3&amp;""", """&amp;TEXT(J3,"aaaa-mm-jj")&amp;""", "&amp;L3&amp;", "&amp;N3&amp;", "&amp;P3&amp;");"</f>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("macarthur", "leon", "121,bd gambetta", "calais", 62100, "03-21-30-65-09", "2014-09-01", "M", "1994-04-12", 3, 1, 2);</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>80</v>
@@ -1738,11 +1741,11 @@
       </c>
       <c r="AV3">
         <f t="shared" ref="AV3:AV11" ca="1" si="9">RANDBETWEEN(0,20)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AW3" t="str">
         <f t="shared" ref="AW3:AW11" ca="1" si="10">"INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES ("&amp;AT3&amp;", "&amp;AU3&amp;", "&amp;AV3&amp;");"</f>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (1, 3, 1);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (1, 3, 4);</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
@@ -1780,7 +1783,7 @@
         <v>80</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L3:L19" si="11">VLOOKUP(K4,$S$2:$V$6,4,FALSE)</f>
+        <f t="shared" ref="L4:L19" si="11">VLOOKUP(K4,$S$2:$V$6,4,FALSE)</f>
         <v>2</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -1799,7 +1802,7 @@
       </c>
       <c r="Q4" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "luc", "9,rue des prairies", "boulogne", 62200, "21-30-20-10", "2014-09-01", "M", "1997-03-12", 2, 2, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "luc", "9,rue des prairies", "boulogne", 62200, "03-21-30-20-10", "2014-09-01", "M", "1997-03-12", 2, 2, 2);</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>81</v>
@@ -1869,11 +1872,11 @@
       </c>
       <c r="AV4">
         <f t="shared" ca="1" si="9"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AW4" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (11, 1, 19);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (11, 1, 11);</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
@@ -1930,7 +1933,7 @@
       </c>
       <c r="Q5" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "sophie", "12,rue des capucines", "wimereux", 62930, "21-89-04-30", "2014-09-01", "F", "1996-03-21", 5, 4, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "sophie", "12,rue des capucines", "wimereux", 62930, "03-21-89-04-30", "2014-09-01", "F", "1996-03-21", 5, 4, 2);</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>87</v>
@@ -1980,11 +1983,11 @@
       </c>
       <c r="AV5">
         <f t="shared" ca="1" si="9"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="AW5" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (12, 3, 11);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (12, 3, 17);</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
@@ -2041,7 +2044,7 @@
       </c>
       <c r="Q6" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "marc", "67,allee ronde", "marcq", 62300, "21-90-87-65", "2014-09-01", "M", "1993-02-05", 3, 1, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("minol", "marc", "67,allee ronde", "marcq", 62300, "03-21-90-87-65", "2014-09-01", "M", "1993-02-05", 3, 1, 2);</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>88</v>
@@ -2078,11 +2081,11 @@
       </c>
       <c r="AV6">
         <f t="shared" ca="1" si="9"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="AW6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (3, 1, 3);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (3, 1, 17);</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
@@ -2139,7 +2142,7 @@
       </c>
       <c r="Q7" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("vendraux", "marc", "5,rue de marseille", "calais", 62100, "21-96-00-09", "2013-09-01", "M", "1996-01-21", 4, 1, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("vendraux", "marc", "5,rue de marseille", "calais", 62100, "03-21-96-00-09", "2013-09-01", "M", "1996-01-21", 4, 1, 2);</v>
       </c>
       <c r="AP7">
         <v>2</v>
@@ -2159,11 +2162,11 @@
       </c>
       <c r="AV7">
         <f t="shared" ca="1" si="9"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="AW7" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (15, 2, 17);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (15, 2, 9);</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
@@ -2220,7 +2223,7 @@
       </c>
       <c r="Q8" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("vendermaele", "helene", "456,rue de paris", "boulogne", 62200, "21-45-45-60", "2014-09-01", "F", "1995-03-30", 5, 2, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("vendermaele", "helene", "456,rue de paris", "boulogne", 62200, "03-21-45-45-60", "2014-09-01", "F", "1995-03-30", 5, 2, 2);</v>
       </c>
       <c r="AP8">
         <v>1</v>
@@ -2240,11 +2243,11 @@
       </c>
       <c r="AV8">
         <f t="shared" ca="1" si="9"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AW8" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (8, 1, 20);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (8, 1, 3);</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
@@ -2301,7 +2304,7 @@
       </c>
       <c r="Q9" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("besson", "loic", "3,allee carpentier", "dunkerque", 59300, "28-90-89-78", "2014-09-01", "M", "1994-05-21", 1, 3, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("besson", "loic", "3,allee carpentier", "dunkerque", 59300, "03-28-90-89-78", "2014-09-01", "M", "1994-05-21", 1, 3, 1);</v>
       </c>
       <c r="AP9">
         <v>2</v>
@@ -2321,11 +2324,11 @@
       </c>
       <c r="AV9">
         <f t="shared" ca="1" si="9"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AW9" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (16, 2, 14);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (16, 2, 6);</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
@@ -2382,7 +2385,7 @@
       </c>
       <c r="Q10" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("godart", "jean-paul", "123,rue de lens", "marck", 59870, "28-09-87-65", "2013-09-01", "M", "1993-01-12", 1, 3, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("godart", "jean-paul", "123,rue de lens", "marck", 59870, "03-28-09-87-65", "2013-09-01", "M", "1993-01-12", 1, 3, 1);</v>
       </c>
       <c r="AP10">
         <v>2</v>
@@ -2402,11 +2405,11 @@
       </c>
       <c r="AV10">
         <f t="shared" ca="1" si="9"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AW10" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (14, 3, 18);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (14, 3, 0);</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
@@ -2463,7 +2466,7 @@
       </c>
       <c r="Q11" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("beaux", "marie", "1,allee des cygnes", "dunkerque", 59100, "21-30-87-90", "2014-09-01", "F", "1996-04-12", 2, 2, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("beaux", "marie", "1,allee des cygnes", "dunkerque", 59100, "03-21-30-87-90", "2014-09-01", "F", "1996-04-12", 2, 2, 2);</v>
       </c>
       <c r="AP11">
         <v>3</v>
@@ -2483,11 +2486,11 @@
       </c>
       <c r="AV11">
         <f t="shared" ca="1" si="9"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AW11" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (9, 1, 8);</v>
+        <v>INSERT INTO Suivis (idStagiaire, idMatiere, note) VALUES (9, 1, 20);</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
@@ -2544,7 +2547,7 @@
       </c>
       <c r="Q12" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("turini", "elsa", "12,route de paris", "boulogne", 62200, "21-32-47-97", "2014-09-01", "F", "1996-07-17", 1, 3, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("turini", "elsa", "12,route de paris", "boulogne", 62200, "03-21-32-47-97", "2014-09-01", "F", "1996-07-17", 1, 3, 2);</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
@@ -2601,7 +2604,7 @@
       </c>
       <c r="Q13" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("torelle", "elise", "123,vallee du denacre", "boulogne", 62200, "21-67-86-90", "2014-09-01", "F", "1997-04-16", 3, 1, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("torelle", "elise", "123,vallee du denacre", "boulogne", 62200, "03-21-67-86-90", "2014-09-01", "F", "1997-04-16", 3, 1, 1);</v>
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
@@ -2658,7 +2661,7 @@
       </c>
       <c r="Q14" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("pharis", "pierre", "12,avenue foch", "calais", 62100, "21-21-85-90", "2014-09-01", "M", "1996-03-18", 4, 1, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("pharis", "pierre", "12,avenue foch", "calais", 62100, "03-21-21-85-90", "2014-09-01", "M", "1996-03-18", 4, 1, 1);</v>
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
@@ -2715,7 +2718,7 @@
       </c>
       <c r="Q15" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("ephyre", "luc", "12,rue de lyon", "calais", 62100, "21-35-32-90", "2014-09-01", "M", "1995-01-21", 3, 4, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("ephyre", "luc", "12,rue de lyon", "calais", 62100, "03-21-35-32-90", "2014-09-01", "M", "1995-01-21", 3, 4, 1);</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
@@ -2772,7 +2775,7 @@
       </c>
       <c r="Q16" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("leclercq", "jules", "12,allee des ravins", "boulogne", 62200, "21-36-71-92", "2014-09-01", "M", "1994-05-19", 3, 1, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("leclercq", "jules", "12,allee des ravins", "boulogne", 62200, "03-21-36-71-92", "2014-09-01", "M", "1994-05-19", 3, 1, 2);</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -2829,7 +2832,7 @@
       </c>
       <c r="Q17" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("dupont", "luc", "21,avenue monsigny", "calais", 62200, "21-21-34-99", "2014-09-01", "M", "1996-11-02", 2, 2, 2);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("dupont", "luc", "21,avenue monsigny", "calais", 62200, "03-21-21-34-99", "2014-09-01", "M", "1996-11-02", 2, 2, 2);</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2886,7 +2889,7 @@
       </c>
       <c r="Q18" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("marke", "loic", "312,route de paris", "wimereux", 62930, "21-87-87-71", "2014-09-01", "M", "1996-11-12", 5, 4, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("marke", "loic", "312,route de paris", "wimereux", 62930, "03-21-87-87-71", "2014-09-01", "M", "1996-11-12", 5, 4, 1);</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2943,7 +2946,7 @@
       </c>
       <c r="Q19" s="13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("dewa", "leon", "121,allee des eglantines", "dunkerque", 59100, "28-30-87-90", "2014-09-01", "M", "1997-04-03", 2, 4, 1);</v>
+        <v>INSERT INTO Stagiaires (nomStagiaire, prenomStagiaire, adresseStagiaire, ville, codePostal, telStagiaire, dateEntree, genreStagiaire, dateNaissance, idFormation, idFormateur, idHebergement) VALUES ("dewa", "leon", "121,allee des eglantines", "dunkerque", 59100, "03-28-30-87-90", "2014-09-01", "M", "1997-04-03", 2, 4, 1);</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>